<commit_message>
map drag & code iteration
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -46,13 +46,25 @@
     <t>Energy</t>
   </si>
   <si>
+    <t>Resource</t>
+  </si>
+  <si>
     <t>大红</t>
   </si>
   <si>
+    <t>player_dahong</t>
+  </si>
+  <si>
     <t>幻影</t>
   </si>
   <si>
+    <t>player_huanying</t>
+  </si>
+  <si>
     <t>迷彩</t>
+  </si>
+  <si>
+    <t>player_micai</t>
   </si>
 </sst>
 </file>
@@ -1197,15 +1209,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1236,13 +1248,16 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>300</v>
@@ -1268,13 +1283,16 @@
       <c r="J2">
         <v>2</v>
       </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -1300,13 +1318,16 @@
       <c r="J3">
         <v>2</v>
       </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -1331,6 +1352,9 @@
       </c>
       <c r="J4">
         <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update team Info page
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -49,22 +49,106 @@
     <t>Resource</t>
   </si>
   <si>
+    <t>Desc</t>
+  </si>
+  <si>
     <t>大红</t>
   </si>
   <si>
     <t>player_dahong</t>
   </si>
   <si>
+    <t>大红的描述测试</t>
+  </si>
+  <si>
     <t>幻影</t>
   </si>
   <si>
     <t>player_huanying</t>
   </si>
   <si>
+    <t>幻影的描述测试</t>
+  </si>
+  <si>
     <t>迷彩</t>
   </si>
   <si>
     <t>player_micai</t>
+  </si>
+  <si>
+    <t>迷彩的描述测试</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test1的描述测试</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test2的描述测试</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test3的描述测试</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test4的描述测试</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test5的描述测试</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test6的描述测试</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test7的描述测试</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test8的描述测试</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test9的描述测试</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test10的描述测试</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test11的描述测试</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test12的描述测试</t>
   </si>
 </sst>
 </file>
@@ -1209,15 +1293,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1251,13 +1335,16 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>300</v>
@@ -1284,15 +1371,18 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -1319,15 +1409,18 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -1354,7 +1447,466 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>110</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
         <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>110</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>90</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>300</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>110</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>90</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>110</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>111</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>500</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>90</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ai logic with EnqueueAction
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Lucky</t>
-  </si>
-  <si>
-    <t>Taunt</t>
   </si>
   <si>
     <t>Resource</t>
@@ -1342,20 +1339,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="N1" sqref="N$1:N$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="14" max="14" width="8.32692307692308" customWidth="1"/>
-    <col min="15" max="15" width="19.3942307692308" customWidth="1"/>
-    <col min="16" max="16" width="53.2019230769231" customWidth="1"/>
+    <col min="14" max="14" width="19.3942307692308" customWidth="1"/>
+    <col min="15" max="15" width="53.2019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1413,16 +1409,13 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1457,34 +1450,31 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>150</v>
+      <c r="N2" t="s">
+        <v>20</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S2">
-        <v>4</v>
-      </c>
-      <c r="T2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1519,34 +1509,31 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3">
-        <v>100</v>
+      <c r="N3" t="s">
+        <v>23</v>
       </c>
       <c r="O3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3">
+        <v>12</v>
+      </c>
+      <c r="S3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
-      </c>
-      <c r="Q3">
-        <v>10</v>
-      </c>
-      <c r="R3">
-        <v>11</v>
-      </c>
-      <c r="S3">
-        <v>12</v>
-      </c>
-      <c r="T3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1581,34 +1568,31 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4">
-        <v>200</v>
+      <c r="N4" t="s">
+        <v>26</v>
       </c>
       <c r="O4" t="s">
         <v>27</v>
       </c>
-      <c r="P4" t="s">
-        <v>28</v>
+      <c r="P4">
+        <v>14</v>
       </c>
       <c r="Q4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S4">
-        <v>16</v>
-      </c>
-      <c r="T4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1643,14 +1627,14 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5">
-        <v>150</v>
+      <c r="N5" t="s">
+        <v>20</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="P5">
+        <v>-1</v>
       </c>
       <c r="Q5">
         <v>-1</v>
@@ -1661,16 +1645,13 @@
       <c r="S5">
         <v>-1</v>
       </c>
-      <c r="T5">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1705,14 +1686,14 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
-        <v>150</v>
+      <c r="N6" t="s">
+        <v>23</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="P6">
+        <v>-1</v>
       </c>
       <c r="Q6">
         <v>-1</v>
@@ -1723,16 +1704,13 @@
       <c r="S6">
         <v>-1</v>
       </c>
-      <c r="T6">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1767,14 +1745,14 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>150</v>
+      <c r="N7" t="s">
+        <v>26</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="P7">
+        <v>-1</v>
       </c>
       <c r="Q7">
         <v>-1</v>
@@ -1785,16 +1763,13 @@
       <c r="S7">
         <v>-1</v>
       </c>
-      <c r="T7">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1829,14 +1804,14 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8">
-        <v>100</v>
+      <c r="N8" t="s">
+        <v>20</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="P8">
+        <v>-1</v>
       </c>
       <c r="Q8">
         <v>-1</v>
@@ -1847,16 +1822,13 @@
       <c r="S8">
         <v>-1</v>
       </c>
-      <c r="T8">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1891,14 +1863,14 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9">
-        <v>200</v>
+      <c r="N9" t="s">
+        <v>23</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="P9">
+        <v>-1</v>
       </c>
       <c r="Q9">
         <v>-1</v>
@@ -1909,16 +1881,13 @@
       <c r="S9">
         <v>-1</v>
       </c>
-      <c r="T9">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1953,14 +1922,14 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10">
-        <v>100</v>
+      <c r="N10" t="s">
+        <v>26</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="P10">
+        <v>-1</v>
       </c>
       <c r="Q10">
         <v>-1</v>
@@ -1971,16 +1940,13 @@
       <c r="S10">
         <v>-1</v>
       </c>
-      <c r="T10">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2015,14 +1981,14 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11">
-        <v>100</v>
+      <c r="N11" t="s">
+        <v>20</v>
       </c>
       <c r="O11" t="s">
-        <v>21</v>
-      </c>
-      <c r="P11" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
       </c>
       <c r="Q11">
         <v>-1</v>
@@ -2033,16 +1999,13 @@
       <c r="S11">
         <v>-1</v>
       </c>
-      <c r="T11">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2077,14 +2040,14 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12">
-        <v>200</v>
+      <c r="N12" t="s">
+        <v>23</v>
       </c>
       <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="P12">
+        <v>-1</v>
       </c>
       <c r="Q12">
         <v>-1</v>
@@ -2095,16 +2058,13 @@
       <c r="S12">
         <v>-1</v>
       </c>
-      <c r="T12">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2139,14 +2099,14 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13">
-        <v>100</v>
+      <c r="N13" t="s">
+        <v>26</v>
       </c>
       <c r="O13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
       </c>
       <c r="Q13">
         <v>-1</v>
@@ -2157,16 +2117,13 @@
       <c r="S13">
         <v>-1</v>
       </c>
-      <c r="T13">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2201,14 +2158,14 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14">
-        <v>100</v>
+      <c r="N14" t="s">
+        <v>20</v>
       </c>
       <c r="O14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="P14">
+        <v>-1</v>
       </c>
       <c r="Q14">
         <v>-1</v>
@@ -2219,16 +2176,13 @@
       <c r="S14">
         <v>-1</v>
       </c>
-      <c r="T14">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2263,14 +2217,14 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15">
-        <v>150</v>
+      <c r="N15" t="s">
+        <v>23</v>
       </c>
       <c r="O15" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="P15">
+        <v>-1</v>
       </c>
       <c r="Q15">
         <v>-1</v>
@@ -2281,16 +2235,13 @@
       <c r="S15">
         <v>-1</v>
       </c>
-      <c r="T15">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2325,14 +2276,14 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16">
-        <v>150</v>
+      <c r="N16" t="s">
+        <v>26</v>
       </c>
       <c r="O16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P16" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="P16">
+        <v>-1</v>
       </c>
       <c r="Q16">
         <v>-1</v>
@@ -2343,16 +2294,13 @@
       <c r="S16">
         <v>-1</v>
       </c>
-      <c r="T16">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -2387,14 +2335,14 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17">
-        <v>200</v>
+      <c r="N17" t="s">
+        <v>26</v>
       </c>
       <c r="O17" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="P17">
+        <v>-1</v>
       </c>
       <c r="Q17">
         <v>-1</v>
@@ -2405,16 +2353,13 @@
       <c r="S17">
         <v>-1</v>
       </c>
-      <c r="T17">
-        <v>-1</v>
-      </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -2449,14 +2394,14 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="N18">
-        <v>200</v>
+      <c r="N18" t="s">
+        <v>26</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="P18">
+        <v>-1</v>
       </c>
       <c r="Q18">
         <v>-1</v>
@@ -2465,9 +2410,6 @@
         <v>-1</v>
       </c>
       <c r="S18">
-        <v>-1</v>
-      </c>
-      <c r="T18">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish restaurant page logic(bugs remain)
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>MaxHungry</t>
   </si>
   <si>
     <t>MaxHP</t>
@@ -1339,19 +1342,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N$1:N$1048576"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="14" max="14" width="19.3942307692308" customWidth="1"/>
-    <col min="15" max="15" width="53.2019230769231" customWidth="1"/>
+    <col min="15" max="15" width="19.3942307692308" customWidth="1"/>
+    <col min="16" max="16" width="53.2019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1409,13 +1412,16 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1424,57 +1430,60 @@
         <v>3</v>
       </c>
       <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
         <v>350</v>
-      </c>
-      <c r="F2">
-        <v>20</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>100</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
       <c r="L2">
         <v>2</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2">
-        <v>0</v>
+      <c r="P2" t="s">
+        <v>22</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>4</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1483,116 +1492,122 @@
         <v>3</v>
       </c>
       <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
         <v>250</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>15</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>110</v>
       </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
       <c r="L3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
       </c>
       <c r="O3" t="s">
         <v>24</v>
       </c>
-      <c r="P3">
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3">
         <v>10</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>11</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>12</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <v>450</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
         <v>25</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>450</v>
-      </c>
-      <c r="F4">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>25</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>90</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
       <c r="L4">
         <v>2</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
       </c>
       <c r="O4" t="s">
         <v>27</v>
       </c>
-      <c r="P4">
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4">
         <v>14</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>15</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>16</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1601,40 +1616,40 @@
         <v>3</v>
       </c>
       <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
         <v>300</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
       </c>
       <c r="G5">
         <v>20</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>100</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5">
-        <v>-1</v>
+        <v>21</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
       </c>
       <c r="Q5">
         <v>-1</v>
@@ -1645,13 +1660,16 @@
       <c r="S5">
         <v>-1</v>
       </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1660,40 +1678,40 @@
         <v>3</v>
       </c>
       <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
         <v>300</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>25</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>110</v>
       </c>
-      <c r="K6">
-        <v>3</v>
-      </c>
       <c r="L6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6">
-        <v>-1</v>
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>32</v>
       </c>
       <c r="Q6">
         <v>-1</v>
@@ -1704,13 +1722,16 @@
       <c r="S6">
         <v>-1</v>
       </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1719,40 +1740,40 @@
         <v>3</v>
       </c>
       <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
         <v>250</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>25</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>90</v>
       </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
       <c r="L7">
         <v>2</v>
       </c>
       <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P7">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>34</v>
       </c>
       <c r="Q7">
         <v>-1</v>
@@ -1763,13 +1784,16 @@
       <c r="S7">
         <v>-1</v>
       </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1778,40 +1802,40 @@
         <v>3</v>
       </c>
       <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
         <v>200</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
       </c>
       <c r="G8">
         <v>20</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>100</v>
       </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
       <c r="L8">
         <v>2</v>
       </c>
       <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8">
-        <v>-1</v>
+        <v>21</v>
+      </c>
+      <c r="P8" t="s">
+        <v>36</v>
       </c>
       <c r="Q8">
         <v>-1</v>
@@ -1822,13 +1846,16 @@
       <c r="S8">
         <v>-1</v>
       </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1837,40 +1864,40 @@
         <v>3</v>
       </c>
       <c r="E9">
+        <v>120</v>
+      </c>
+      <c r="F9">
         <v>500</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>25</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>15</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>110</v>
       </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
       <c r="L9">
         <v>2</v>
       </c>
       <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9">
-        <v>-1</v>
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>38</v>
       </c>
       <c r="Q9">
         <v>-1</v>
@@ -1881,13 +1908,16 @@
       <c r="S9">
         <v>-1</v>
       </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1896,40 +1926,40 @@
         <v>3</v>
       </c>
       <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
         <v>300</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>15</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>25</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>90</v>
       </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
       <c r="L10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P10" t="s">
+        <v>40</v>
       </c>
       <c r="Q10">
         <v>-1</v>
@@ -1940,13 +1970,16 @@
       <c r="S10">
         <v>-1</v>
       </c>
+      <c r="T10">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1955,40 +1988,40 @@
         <v>3</v>
       </c>
       <c r="E11">
+        <v>80</v>
+      </c>
+      <c r="F11">
         <v>250</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
       </c>
       <c r="G11">
         <v>20</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>100</v>
       </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
       <c r="L11">
         <v>2</v>
       </c>
       <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>41</v>
-      </c>
-      <c r="P11">
-        <v>-1</v>
+        <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>42</v>
       </c>
       <c r="Q11">
         <v>-1</v>
@@ -1999,13 +2032,16 @@
       <c r="S11">
         <v>-1</v>
       </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2014,40 +2050,40 @@
         <v>3</v>
       </c>
       <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
         <v>400</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>25</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>15</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>110</v>
       </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
       <c r="L12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>43</v>
-      </c>
-      <c r="P12">
-        <v>-1</v>
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>44</v>
       </c>
       <c r="Q12">
         <v>-1</v>
@@ -2058,13 +2094,16 @@
       <c r="S12">
         <v>-1</v>
       </c>
+      <c r="T12">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2073,40 +2112,40 @@
         <v>3</v>
       </c>
       <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
         <v>200</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>15</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>25</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>90</v>
       </c>
-      <c r="K13">
-        <v>2</v>
-      </c>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>46</v>
       </c>
       <c r="Q13">
         <v>-1</v>
@@ -2117,13 +2156,16 @@
       <c r="S13">
         <v>-1</v>
       </c>
+      <c r="T13">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2132,40 +2174,40 @@
         <v>3</v>
       </c>
       <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
         <v>200</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
       </c>
       <c r="G14">
         <v>20</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>100</v>
       </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
       <c r="L14">
         <v>2</v>
       </c>
       <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>47</v>
-      </c>
-      <c r="P14">
-        <v>-1</v>
+        <v>21</v>
+      </c>
+      <c r="P14" t="s">
+        <v>48</v>
       </c>
       <c r="Q14">
         <v>-1</v>
@@ -2176,13 +2218,16 @@
       <c r="S14">
         <v>-1</v>
       </c>
+      <c r="T14">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2191,40 +2236,40 @@
         <v>3</v>
       </c>
       <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
         <v>350</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>25</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>15</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>110</v>
       </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
       <c r="L15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>49</v>
-      </c>
-      <c r="P15">
-        <v>-1</v>
+        <v>24</v>
+      </c>
+      <c r="P15" t="s">
+        <v>50</v>
       </c>
       <c r="Q15">
         <v>-1</v>
@@ -2235,13 +2280,16 @@
       <c r="S15">
         <v>-1</v>
       </c>
+      <c r="T15">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2250,40 +2298,40 @@
         <v>3</v>
       </c>
       <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
         <v>400</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>20</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>10</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>90</v>
       </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
       <c r="L16">
         <v>2</v>
       </c>
       <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>51</v>
-      </c>
-      <c r="P16">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P16" t="s">
+        <v>52</v>
       </c>
       <c r="Q16">
         <v>-1</v>
@@ -2294,13 +2342,16 @@
       <c r="S16">
         <v>-1</v>
       </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -2309,40 +2360,40 @@
         <v>3</v>
       </c>
       <c r="E17">
+        <v>120</v>
+      </c>
+      <c r="F17">
         <v>450</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>15</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>25</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>90</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
       <c r="L17">
         <v>2</v>
       </c>
       <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>53</v>
-      </c>
-      <c r="P17">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P17" t="s">
+        <v>54</v>
       </c>
       <c r="Q17">
         <v>-1</v>
@@ -2353,13 +2404,16 @@
       <c r="S17">
         <v>-1</v>
       </c>
+      <c r="T17">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -2368,40 +2422,40 @@
         <v>3</v>
       </c>
       <c r="E18">
+        <v>120</v>
+      </c>
+      <c r="F18">
         <v>450</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>15</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>25</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>90</v>
       </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
       <c r="L18">
         <v>2</v>
       </c>
       <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>55</v>
-      </c>
-      <c r="P18">
-        <v>-1</v>
+        <v>27</v>
+      </c>
+      <c r="P18" t="s">
+        <v>56</v>
       </c>
       <c r="Q18">
         <v>-1</v>
@@ -2410,6 +2464,9 @@
         <v>-1</v>
       </c>
       <c r="S18">
+        <v>-1</v>
+      </c>
+      <c r="T18">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add bar page logic
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Race</t>
+  </si>
+  <si>
     <t>Job</t>
   </si>
   <si>
@@ -71,6 +74,18 @@
     <t>Lucky</t>
   </si>
   <si>
+    <t>MaxHPFloat</t>
+  </si>
+  <si>
+    <t>StrengthFloat</t>
+  </si>
+  <si>
+    <t>DefenseFloat</t>
+  </si>
+  <si>
+    <t>SpeedFloat</t>
+  </si>
+  <si>
     <t>Resource</t>
   </si>
   <si>
@@ -116,85 +131,85 @@
     <t>迷彩的描述测试</t>
   </si>
   <si>
-    <t>赵云</t>
+    <t>游隼</t>
   </si>
   <si>
     <t>赵云的描述测试</t>
   </si>
   <si>
-    <t>关羽</t>
+    <t>鸵鸟</t>
   </si>
   <si>
     <t>关羽的描述测试</t>
   </si>
   <si>
-    <t>黄忠</t>
+    <t>啄木鸟</t>
   </si>
   <si>
     <t>黄忠的描述测试</t>
   </si>
   <si>
-    <t>刘备</t>
+    <t>鹦鹉</t>
   </si>
   <si>
     <t>刘备的描述测试</t>
   </si>
   <si>
-    <t>张飞</t>
+    <t>金雕</t>
   </si>
   <si>
     <t>张飞的描述测试</t>
   </si>
   <si>
-    <t>马超</t>
+    <t>鹈鹕</t>
   </si>
   <si>
     <t>马超的描述测试</t>
   </si>
   <si>
-    <t>曹操</t>
+    <t>白鹳</t>
   </si>
   <si>
     <t>曹操的描述测试</t>
   </si>
   <si>
-    <t>孙权</t>
+    <t>丹顶鹤</t>
   </si>
   <si>
     <t>孙权的描述测试</t>
   </si>
   <si>
-    <t>诸葛亮</t>
+    <t>火烈鸟</t>
   </si>
   <si>
     <t>诸葛亮的描述测试</t>
   </si>
   <si>
-    <t>庞统</t>
+    <t>杜鹃</t>
   </si>
   <si>
     <t>庞统的描述测试</t>
   </si>
   <si>
-    <t>吕布</t>
+    <t>夜莺</t>
   </si>
   <si>
     <t>吕布的描述测试</t>
   </si>
   <si>
-    <t>典韦</t>
+    <t>布谷</t>
   </si>
   <si>
     <t>典韦的描述测试</t>
   </si>
   <si>
-    <t>许褚</t>
+    <t>蜂鸟</t>
   </si>
   <si>
     <t>许褚的描述测试</t>
   </si>
   <si>
-    <t>庞德</t>
+    <t>信天翁</t>
   </si>
   <si>
     <t>庞德的描述测试</t>
@@ -1342,19 +1357,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="15" max="15" width="19.3942307692308" customWidth="1"/>
-    <col min="16" max="16" width="53.2019230769231" customWidth="1"/>
+    <col min="16" max="16" width="12.1730769230769" customWidth="1"/>
+    <col min="17" max="18" width="12.8173076923077" customWidth="1"/>
+    <col min="19" max="19" width="10.4134615384615" customWidth="1"/>
+    <col min="20" max="20" width="19.3942307692308" customWidth="1"/>
+    <col min="21" max="21" width="53.2019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1415,1058 +1433,1277 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>100</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>350</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
       </c>
       <c r="H2">
         <v>20</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>100</v>
       </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
       <c r="M2">
         <v>2</v>
       </c>
       <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>1</v>
       </c>
-      <c r="S2">
+      <c r="X2">
         <v>4</v>
       </c>
-      <c r="T2">
+      <c r="Y2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>80</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>250</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>25</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>15</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>110</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>3</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
       <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3">
+        <v>10</v>
+      </c>
+      <c r="W3">
         <v>11</v>
       </c>
-      <c r="S3">
+      <c r="X3">
         <v>12</v>
       </c>
-      <c r="T3">
+      <c r="Y3">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>120</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>450</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>15</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>25</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>90</v>
       </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
       <c r="M4">
         <v>2</v>
       </c>
       <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4">
         <v>14</v>
       </c>
-      <c r="R4">
+      <c r="W4">
         <v>15</v>
       </c>
-      <c r="S4">
+      <c r="X4">
         <v>16</v>
       </c>
-      <c r="T4">
+      <c r="Y4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>100</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>100</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>300</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
       </c>
       <c r="H5">
         <v>20</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>100</v>
       </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
       <c r="M5">
         <v>2</v>
       </c>
       <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>20</v>
       </c>
       <c r="Q5">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R5">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S5">
-        <v>-1</v>
-      </c>
-      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="T5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5">
+        <v>-1</v>
+      </c>
+      <c r="W5">
+        <v>-1</v>
+      </c>
+      <c r="X5">
+        <v>-1</v>
+      </c>
+      <c r="Y5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>101</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>300</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>25</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>15</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>110</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>3</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
       <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S6">
-        <v>-1</v>
-      </c>
-      <c r="T6">
+        <v>10</v>
+      </c>
+      <c r="T6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6">
+        <v>-1</v>
+      </c>
+      <c r="W6">
+        <v>-1</v>
+      </c>
+      <c r="X6">
+        <v>-1</v>
+      </c>
+      <c r="Y6">
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>102</v>
       </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>250</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>15</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>25</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>90</v>
       </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
       <c r="M7">
         <v>2</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" t="s">
-        <v>34</v>
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>20</v>
       </c>
       <c r="Q7">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R7">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S7">
-        <v>-1</v>
-      </c>
-      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="T7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7">
+        <v>-1</v>
+      </c>
+      <c r="W7">
+        <v>-1</v>
+      </c>
+      <c r="X7">
+        <v>-1</v>
+      </c>
+      <c r="Y7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>103</v>
       </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>40</v>
       </c>
       <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>80</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>200</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
       </c>
       <c r="H8">
         <v>20</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>100</v>
       </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
       <c r="M8">
         <v>2</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>20</v>
       </c>
       <c r="Q8">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R8">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S8">
-        <v>-1</v>
-      </c>
-      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="T8" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" t="s">
+        <v>41</v>
+      </c>
+      <c r="V8">
+        <v>-1</v>
+      </c>
+      <c r="W8">
+        <v>-1</v>
+      </c>
+      <c r="X8">
+        <v>-1</v>
+      </c>
+      <c r="Y8">
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>500</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>25</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>15</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>110</v>
       </c>
-      <c r="L9">
-        <v>2</v>
-      </c>
       <c r="M9">
         <v>2</v>
       </c>
       <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>20</v>
       </c>
       <c r="Q9">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R9">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S9">
-        <v>-1</v>
-      </c>
-      <c r="T9">
+        <v>10</v>
+      </c>
+      <c r="T9" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" t="s">
+        <v>43</v>
+      </c>
+      <c r="V9">
+        <v>-1</v>
+      </c>
+      <c r="W9">
+        <v>-1</v>
+      </c>
+      <c r="X9">
+        <v>-1</v>
+      </c>
+      <c r="Y9">
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>105</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>100</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>300</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>15</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>25</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>90</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="M10">
-        <v>2</v>
-      </c>
       <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>20</v>
       </c>
       <c r="Q10">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R10">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S10">
-        <v>-1</v>
-      </c>
-      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="T10" t="s">
+        <v>32</v>
+      </c>
+      <c r="U10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10">
+        <v>-1</v>
+      </c>
+      <c r="W10">
+        <v>-1</v>
+      </c>
+      <c r="X10">
+        <v>-1</v>
+      </c>
+      <c r="Y10">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>106</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
+      <c r="C11" t="s">
+        <v>46</v>
       </c>
       <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>80</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>250</v>
-      </c>
-      <c r="G11">
-        <v>20</v>
       </c>
       <c r="H11">
         <v>20</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>100</v>
       </c>
-      <c r="L11">
-        <v>2</v>
-      </c>
       <c r="M11">
         <v>2</v>
       </c>
       <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>21</v>
-      </c>
-      <c r="P11" t="s">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>20</v>
       </c>
       <c r="Q11">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R11">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S11">
-        <v>-1</v>
-      </c>
-      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="T11" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" t="s">
+        <v>47</v>
+      </c>
+      <c r="V11">
+        <v>-1</v>
+      </c>
+      <c r="W11">
+        <v>-1</v>
+      </c>
+      <c r="X11">
+        <v>-1</v>
+      </c>
+      <c r="Y11">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>107</v>
       </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
+      <c r="C12" t="s">
+        <v>48</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
         <v>120</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>400</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>25</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>15</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>110</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>3</v>
       </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
       <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>20</v>
       </c>
       <c r="Q12">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R12">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S12">
-        <v>-1</v>
-      </c>
-      <c r="T12">
+        <v>10</v>
+      </c>
+      <c r="T12" t="s">
+        <v>29</v>
+      </c>
+      <c r="U12" t="s">
+        <v>49</v>
+      </c>
+      <c r="V12">
+        <v>-1</v>
+      </c>
+      <c r="W12">
+        <v>-1</v>
+      </c>
+      <c r="X12">
+        <v>-1</v>
+      </c>
+      <c r="Y12">
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>108</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
+      <c r="C13" t="s">
+        <v>50</v>
       </c>
       <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>80</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>200</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>15</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>25</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>90</v>
       </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
       <c r="M13">
         <v>2</v>
       </c>
       <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
       </c>
       <c r="Q13">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R13">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S13">
-        <v>-1</v>
-      </c>
-      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="T13" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" t="s">
+        <v>51</v>
+      </c>
+      <c r="V13">
+        <v>-1</v>
+      </c>
+      <c r="W13">
+        <v>-1</v>
+      </c>
+      <c r="X13">
+        <v>-1</v>
+      </c>
+      <c r="Y13">
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>109</v>
       </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
+      <c r="C14" t="s">
+        <v>52</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>3</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>80</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>200</v>
-      </c>
-      <c r="G14">
-        <v>20</v>
       </c>
       <c r="H14">
         <v>20</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>100</v>
       </c>
-      <c r="L14">
-        <v>2</v>
-      </c>
       <c r="M14">
         <v>2</v>
       </c>
       <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>20</v>
       </c>
       <c r="Q14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R14">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S14">
-        <v>-1</v>
-      </c>
-      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="T14" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" t="s">
+        <v>53</v>
+      </c>
+      <c r="V14">
+        <v>-1</v>
+      </c>
+      <c r="W14">
+        <v>-1</v>
+      </c>
+      <c r="X14">
+        <v>-1</v>
+      </c>
+      <c r="Y14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>110</v>
       </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>100</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>350</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>25</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>15</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>110</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>3</v>
       </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
       <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>20</v>
       </c>
       <c r="Q15">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R15">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S15">
-        <v>-1</v>
-      </c>
-      <c r="T15">
+        <v>10</v>
+      </c>
+      <c r="T15" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15">
+        <v>-1</v>
+      </c>
+      <c r="W15">
+        <v>-1</v>
+      </c>
+      <c r="X15">
+        <v>-1</v>
+      </c>
+      <c r="Y15">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>111</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>100</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>400</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>20</v>
       </c>
-      <c r="H16">
-        <v>10</v>
-      </c>
       <c r="I16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>90</v>
       </c>
-      <c r="L16">
-        <v>2</v>
-      </c>
       <c r="M16">
         <v>2</v>
       </c>
       <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P16" t="s">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>20</v>
       </c>
       <c r="Q16">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R16">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S16">
-        <v>-1</v>
-      </c>
-      <c r="T16">
+        <v>10</v>
+      </c>
+      <c r="T16" t="s">
+        <v>32</v>
+      </c>
+      <c r="U16" t="s">
+        <v>57</v>
+      </c>
+      <c r="V16">
+        <v>-1</v>
+      </c>
+      <c r="W16">
+        <v>-1</v>
+      </c>
+      <c r="X16">
+        <v>-1</v>
+      </c>
+      <c r="Y16">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>112</v>
       </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
+      <c r="C17" t="s">
+        <v>58</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
         <v>120</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>450</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>15</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>25</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>90</v>
       </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
       <c r="M17">
         <v>2</v>
       </c>
       <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" t="s">
-        <v>54</v>
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>20</v>
       </c>
       <c r="Q17">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R17">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S17">
-        <v>-1</v>
-      </c>
-      <c r="T17">
+        <v>10</v>
+      </c>
+      <c r="T17" t="s">
+        <v>32</v>
+      </c>
+      <c r="U17" t="s">
+        <v>59</v>
+      </c>
+      <c r="V17">
+        <v>-1</v>
+      </c>
+      <c r="W17">
+        <v>-1</v>
+      </c>
+      <c r="X17">
+        <v>-1</v>
+      </c>
+      <c r="Y17">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>113</v>
       </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
+      <c r="C18" t="s">
+        <v>60</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
         <v>120</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>450</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>15</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>25</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>90</v>
       </c>
-      <c r="L18">
-        <v>2</v>
-      </c>
       <c r="M18">
         <v>2</v>
       </c>
       <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" t="s">
-        <v>56</v>
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>20</v>
       </c>
       <c r="Q18">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="R18">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S18">
-        <v>-1</v>
-      </c>
-      <c r="T18">
+        <v>10</v>
+      </c>
+      <c r="T18" t="s">
+        <v>32</v>
+      </c>
+      <c r="U18" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18">
+        <v>-1</v>
+      </c>
+      <c r="W18">
+        <v>-1</v>
+      </c>
+      <c r="X18">
+        <v>-1</v>
+      </c>
+      <c r="Y18">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add bar page collect character logic
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="U5" sqref="U5:U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -1534,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>80</v>
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>120</v>
@@ -1682,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -1830,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -1904,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>80</v>
@@ -1978,7 +1978,7 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>120</v>
@@ -2052,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -2126,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>80</v>
@@ -2200,7 +2200,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>120</v>
@@ -2274,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>80</v>
@@ -2348,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>80</v>
@@ -2422,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>100</v>
@@ -2496,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -2570,7 +2570,7 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>120</v>
@@ -2644,7 +2644,7 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>120</v>

</xml_diff>

<commit_message>
bar page logic complete
</commit_message>
<xml_diff>
--- a/Data/CharacterDefine.xlsx
+++ b/Data/CharacterDefine.xlsx
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5:U18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -1534,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>80</v>
@@ -1608,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>120</v>

</xml_diff>